<commit_message>
Update SP Sales Amount Analysis Handling
</commit_message>
<xml_diff>
--- a/src/main/resources/source/enhancement/Open PO Summary.xlsx
+++ b/src/main/resources/source/enhancement/Open PO Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WillShen\OneDrive\MyWorkSpace\ActionPC\P249G3\workspaces\somsInteg\soms\src\main\resources\template\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WillShen\OneDrive\MyWorkSpace\ActionPC\P249G3\workspaces\apache-poi-git\apache-poi\src\main\resources\source\enhancement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD684D50-5AF6-489D-9F7F-2FD2744A018F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC7D933-9F2B-4D2A-BBA8-F012905F5FAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{65DF43ED-97A1-4003-A8B0-81B335E419A5}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="163" r:id="rId3"/>
+    <pivotCache cacheId="152" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +53,7 @@
   </si>
   <si>
     <t>Model</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Project</t>
@@ -61,7 +61,7 @@
   </si>
   <si>
     <t>Part Type</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Order Qty</t>
@@ -78,7 +78,7 @@
   </si>
   <si>
     <t>Original CRD</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Latest CRD</t>
@@ -149,7 +149,7 @@
   </si>
   <si>
     <t>Target ETD Month</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Open PO Age</t>
@@ -219,7 +219,7 @@
   </si>
   <si>
     <t>Open PO Summary</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>PO Status</t>
@@ -265,27 +265,27 @@
   </si>
   <si>
     <t>PRODUCT GROUP</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Region Code</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Supplier Name</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>RO PO Date</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PO Sending Date</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PO Type</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PO Number</t>
@@ -296,11 +296,11 @@
   </si>
   <si>
     <t>Sub Line Number</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PO Status</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>AI Part No.</t>
@@ -315,7 +315,7 @@
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -340,13 +340,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="1"/>
@@ -367,16 +360,37 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="8"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -435,35 +449,47 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -471,33 +497,107 @@
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="千分位" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="64">
     <dxf>
-      <alignment wrapText="0"/>
+      <numFmt numFmtId="22" formatCode="mmm\-yy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="8"/>
+      </font>
     </dxf>
     <dxf>
       <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
@@ -719,9 +819,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="PivotStyle01" table="0" count="3" xr9:uid="{7E057124-D9D6-4375-ABF5-9CC2ECD8F15B}">
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="firstRowStripe" dxfId="50"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="63"/>
+      <tableStyleElement type="firstRowStripe" dxfId="62"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="61"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -13310,7 +13410,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A9F289D0-17D2-43B7-B1E8-806D72D4AD63}" name="樞紐分析表2" cacheId="163" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A9F289D0-17D2-43B7-B1E8-806D72D4AD63}" name="樞紐分析表2" cacheId="152" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="B8:M15" firstHeaderRow="1" firstDataRow="3" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="52">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -13472,52 +13572,52 @@
   <dataFields count="1">
     <dataField name="加總 - Open Qty" fld="21" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="41">
-    <format dxfId="48">
+  <formats count="61">
+    <format dxfId="60">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="59">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="58">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="57">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="56">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="55">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="54">
       <pivotArea field="39" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="53">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="52">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="39" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="39" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0"/>
@@ -13525,7 +13625,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" defaultSubtotal="1"/>
@@ -13533,7 +13633,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0" selected="0"/>
@@ -13542,24 +13642,24 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="44">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -13571,7 +13671,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -13587,7 +13687,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -13599,7 +13699,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -13611,35 +13711,35 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="38">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="37">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="36">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="35">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="34">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="33">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="39" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0"/>
@@ -13647,7 +13747,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0" selected="0"/>
@@ -13656,26 +13756,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="27">
       <pivotArea field="39" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="26">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="25">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -13687,7 +13787,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -13703,7 +13803,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -13715,8 +13815,131 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="20">
+      <pivotArea field="39" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="19">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="18">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="17">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="15">
+      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea field="39" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="39" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0"/>
+          <reference field="39" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="3" count="0"/>
+          <reference field="39" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="7" count="5">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="7" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="7" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="0">
-      <pivotArea field="39" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="39" count="0"/>
+        </references>
+      </pivotArea>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyle01" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
@@ -14030,46 +14253,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF722525-74C7-4197-ACC9-35D56B47CB43}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="20.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="19.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="6"/>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="20.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="14.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5"/>
+      <c r="C5"/>
+    </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>49</v>
       </c>
       <c r="N8" s="8"/>
@@ -14077,20 +14301,20 @@
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
     </row>
-    <row r="9" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="E9" s="6" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="10" t="s">
         <v>44</v>
       </c>
       <c r="N9" s="8"/>
@@ -14098,53 +14322,54 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
     </row>
-    <row r="10" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="7" t="s">
         <v>60</v>
       </c>
+      <c r="M10" s="10"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
     </row>
-    <row r="11" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>61</v>
       </c>
       <c r="E11" s="9">
@@ -14171,8 +14396,9 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
     </row>
-    <row r="12" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="D12" s="6" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="D12" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="9"/>
@@ -14199,8 +14425,9 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
     </row>
-    <row r="13" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="D13" s="6" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="D13" s="7" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="9">
@@ -14225,8 +14452,9 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
     </row>
-    <row r="14" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="D14" s="6" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="D14" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="9">
@@ -14251,8 +14479,8 @@
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
     </row>
-    <row r="15" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="9">
@@ -14287,7 +14515,7 @@
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -14305,7 +14533,7 @@
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="2:17" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -14334,166 +14562,169 @@
   <dimension ref="A1:AZ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>